<commit_message>
more equals sign changes
</commit_message>
<xml_diff>
--- a/ComparisonQG.xlsx
+++ b/ComparisonQG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scaparas\.ssh\wwk-repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169B9D09-97A6-443F-AC92-9F3167E04FB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807474AF-E842-4B4D-894E-D9545771BACD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>La</t>
   </si>
@@ -682,6 +682,27 @@
   </si>
   <si>
     <t>MN15 2nd</t>
+  </si>
+  <si>
+    <t>B3PW91</t>
+  </si>
+  <si>
+    <t>BMK</t>
+  </si>
+  <si>
+    <t>HOMO-&gt;LUMO</t>
+  </si>
+  <si>
+    <t>HOMO-1-&gt;LUMO</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CAM-B3LYP</t>
+  </si>
+  <si>
+    <t>HOMO-&gt;LUMO+1</t>
   </si>
 </sst>
 </file>
@@ -728,7 +749,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +774,18 @@
         <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -1013,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1036,9 +1069,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1050,9 +1080,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1063,26 +1090,69 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1467,14 +1537,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="10" width="11.875" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="10" width="15.125" customWidth="1"/>
     <col min="11" max="11" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1491,38 +1561,38 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30" t="str">
+      <c r="C3" s="24" t="str">
         <f>_xlfn.CONCAT(B3, $R$3)</f>
         <v>APFD 2nd</v>
       </c>
-      <c r="D3" s="30" t="str">
+      <c r="D3" s="24" t="str">
         <f>_xlfn.CONCAT(B3, $R$4)</f>
         <v>APFD 3rd</v>
       </c>
-      <c r="E3" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="30" t="str">
+      <c r="E3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="24" t="str">
         <f>_xlfn.CONCAT(E3, $R$3)</f>
-        <v>APFD 2nd</v>
-      </c>
-      <c r="G3" s="30" t="str">
+        <v>B3PW91 2nd</v>
+      </c>
+      <c r="G3" s="24" t="str">
         <f>_xlfn.CONCAT(E3, $R$4)</f>
-        <v>APFD 3rd</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="30" t="str">
+        <v>B3PW91 3rd</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="24" t="str">
         <f>_xlfn.CONCAT(H3, $R$3)</f>
-        <v>APFD 2nd</v>
-      </c>
-      <c r="J3" s="21" t="str">
+        <v>BMK 2nd</v>
+      </c>
+      <c r="J3" s="19" t="str">
         <f>_xlfn.CONCAT(H3, $R$4)</f>
-        <v>APFD 3rd</v>
+        <v>BMK 3rd</v>
       </c>
       <c r="K3" s="6"/>
       <c r="M3" s="7" t="s">
@@ -1545,26 +1615,38 @@
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="22"/>
+      <c r="B4" s="26">
+        <v>9.6850718265418495E-2</v>
+      </c>
+      <c r="C4" s="27">
+        <v>8.9359946423768405E-2</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.19890472794921099</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.101716223024096</v>
+      </c>
+      <c r="F4" s="39">
+        <v>8.8759156961115401E-2</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0.250777248761264</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="6"/>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="11">
         <v>1.339</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="11">
         <v>1.4159999999999999</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="12">
         <v>1.3480000000000001</v>
       </c>
       <c r="R4" t="s">
@@ -1575,26 +1657,38 @@
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="22"/>
+      <c r="B5" s="31">
+        <v>0.1007</v>
+      </c>
+      <c r="C5" s="30">
+        <v>5.1700000000000003E-2</v>
+      </c>
+      <c r="D5" s="30">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
+        <v>9.3100000000000002E-2</v>
+      </c>
+      <c r="F5" s="30">
+        <v>4.65E-2</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="6"/>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="11">
         <v>1.429</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="11">
         <v>1.3640000000000001</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="12">
         <v>1.4319999999999999</v>
       </c>
     </row>
@@ -1602,59 +1696,83 @@
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="22"/>
+      <c r="B6" s="31">
+        <v>4.9704875334317</v>
+      </c>
+      <c r="C6" s="30">
+        <v>2.5481153349093102</v>
+      </c>
+      <c r="D6" s="30">
+        <v>8.9267585051909997</v>
+      </c>
+      <c r="E6" s="30">
+        <v>5.0514170853335703</v>
+      </c>
+      <c r="F6" s="30">
+        <v>2.5419769668507999</v>
+      </c>
+      <c r="G6" s="30">
+        <v>9.0259077000598609</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="20"/>
       <c r="K6" s="6"/>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="11">
         <v>1.43</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="11">
         <v>1.4419999999999999</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="12">
         <v>1.419</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="23"/>
+      <c r="B7" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="6"/>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="11">
         <v>1.4219999999999999</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="11">
         <v>1.405</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="12">
         <v>1.4279999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="24"/>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="33" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="34"/>
@@ -1663,19 +1781,19 @@
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="15"/>
-      <c r="M8" s="11" t="s">
+      <c r="I8" s="35"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="14"/>
+      <c r="M8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="11">
         <v>1.4279999999999999</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="11">
         <v>1.427</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="12">
         <v>1.4259999999999999</v>
       </c>
     </row>
@@ -1683,49 +1801,49 @@
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="30" t="str">
+      <c r="C9" s="24" t="str">
         <f>_xlfn.CONCAT(B9, $R$3)</f>
         <v>APFD 2nd</v>
       </c>
-      <c r="D9" s="30" t="str">
+      <c r="D9" s="24" t="str">
         <f>_xlfn.CONCAT(B9, $R$4)</f>
         <v>APFD 3rd</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="30" t="str">
+      <c r="E9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="24" t="str">
         <f>_xlfn.CONCAT(E9, $R$3)</f>
-        <v>APFD 2nd</v>
-      </c>
-      <c r="G9" s="30" t="str">
+        <v>B3PW91 2nd</v>
+      </c>
+      <c r="G9" s="24" t="str">
         <f>_xlfn.CONCAT(E9, $R$4)</f>
-        <v>APFD 3rd</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="30" t="str">
+        <v>B3PW91 3rd</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="24" t="str">
         <f>_xlfn.CONCAT(H9, $R$3)</f>
-        <v>APFD 2nd</v>
-      </c>
-      <c r="J9" s="21" t="str">
+        <v>BMK 2nd</v>
+      </c>
+      <c r="J9" s="19" t="str">
         <f>_xlfn.CONCAT(H9, $R$4)</f>
-        <v>APFD 3rd</v>
-      </c>
-      <c r="M9" s="11" t="s">
+        <v>BMK 3rd</v>
+      </c>
+      <c r="M9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="11">
         <v>1.381</v>
       </c>
-      <c r="O9" s="12">
+      <c r="O9" s="11">
         <v>1.413</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="12">
         <v>1.38</v>
       </c>
     </row>
@@ -1733,25 +1851,31 @@
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="13"/>
-      <c r="M10" s="11" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="29">
+        <v>0.139357465356059</v>
+      </c>
+      <c r="F10" s="39">
+        <v>0.10104232488227401</v>
+      </c>
+      <c r="G10" s="39">
+        <v>0.203368013596786</v>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="37"/>
+      <c r="M10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="11">
         <v>1.4430000000000001</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="11">
         <v>1.4159999999999999</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="12">
         <v>1.4530000000000001</v>
       </c>
     </row>
@@ -1759,25 +1883,31 @@
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="13"/>
-      <c r="M11" s="11" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30">
+        <v>9.3915629900000006E-2</v>
+      </c>
+      <c r="F11" s="30">
+        <v>2.2947677400000002E-2</v>
+      </c>
+      <c r="G11" s="30">
+        <v>4.2798997999999996E-3</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="37"/>
+      <c r="M11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="11">
         <v>1.405</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="11">
         <v>1.4139999999999999</v>
       </c>
-      <c r="P11" s="13">
+      <c r="P11" s="12">
         <v>1.3939999999999999</v>
       </c>
     </row>
@@ -1785,103 +1915,159 @@
       <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="13"/>
-      <c r="M12" s="11" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30">
+        <v>2.23264002696359</v>
+      </c>
+      <c r="F12" s="30">
+        <v>2.25923967077421</v>
+      </c>
+      <c r="G12" s="30">
+        <v>2.3289553559482399</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="37"/>
+      <c r="M12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="11">
         <v>1.411</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="11">
         <v>1.345</v>
       </c>
-      <c r="P12" s="13">
+      <c r="P12" s="12">
         <v>1.41</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="18"/>
-      <c r="M13" s="11" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="38"/>
+      <c r="M13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="11">
         <v>1.397</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="11">
         <v>1.46</v>
       </c>
-      <c r="P13" s="13">
+      <c r="P13" s="12">
         <v>1.41</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="M14" s="16" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36"/>
+      <c r="M14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="16">
         <v>1.0109999999999999</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14" s="16">
         <v>1.0089999999999999</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="17">
         <v>1.014</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="24" t="str">
+        <f>_xlfn.CONCAT(B15, $R$3)</f>
+        <v>CAM-B3LYP 2nd</v>
+      </c>
+      <c r="D15" s="24" t="str">
+        <f>_xlfn.CONCAT(B15, $R$4)</f>
+        <v>CAM-B3LYP 3rd</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="24" t="str">
+        <f>_xlfn.CONCAT(E15, $R$3)</f>
+        <v>B3PW91 2nd</v>
+      </c>
+      <c r="G15" s="24" t="str">
+        <f>_xlfn.CONCAT(E15, $R$4)</f>
+        <v>B3PW91 3rd</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="24" t="str">
+        <f>_xlfn.CONCAT(H15, $R$3)</f>
+        <v>BMK 2nd</v>
+      </c>
+      <c r="J15" s="19" t="str">
+        <f>_xlfn.CONCAT(H15, $R$4)</f>
+        <v>BMK 3rd</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="20"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="A17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="20"/>
       <c r="M17" s="7" t="s">
         <v>4</v>
       </c>
@@ -1896,175 +2082,281 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="20"/>
-      <c r="M18" s="11" t="s">
+      <c r="A18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="31"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="20"/>
+      <c r="M18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N18" s="11">
         <v>1.339</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="11">
         <v>1.3360000000000001</v>
       </c>
-      <c r="P18" s="13">
+      <c r="P18" s="12">
         <v>1.3480000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="6"/>
-      <c r="M19" s="11" t="s">
+    <row r="19" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="21"/>
+      <c r="M19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="11">
         <v>1.4279999999999999</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="11">
         <v>1.4430000000000001</v>
       </c>
-      <c r="P19" s="13">
+      <c r="P19" s="12">
         <v>1.4330000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M20" s="11" t="s">
+    <row r="20" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="22"/>
+      <c r="B20" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="36"/>
+      <c r="M20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N20" s="12">
+      <c r="N20" s="11">
         <v>1.43</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="11">
         <v>1.401</v>
       </c>
-      <c r="P20" s="13">
+      <c r="P20" s="12">
         <v>1.42</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M21" s="11" t="s">
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="24" t="str">
+        <f>_xlfn.CONCAT(B21, $R$3)</f>
+        <v>APFD 2nd</v>
+      </c>
+      <c r="D21" s="24" t="str">
+        <f>_xlfn.CONCAT(B21, $R$4)</f>
+        <v>APFD 3rd</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="24" t="str">
+        <f>_xlfn.CONCAT(E21, $R$3)</f>
+        <v>B3PW91 2nd</v>
+      </c>
+      <c r="G21" s="24" t="str">
+        <f>_xlfn.CONCAT(E21, $R$4)</f>
+        <v>B3PW91 3rd</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="24" t="str">
+        <f>_xlfn.CONCAT(H21, $R$3)</f>
+        <v>BMK 2nd</v>
+      </c>
+      <c r="J21" s="19" t="str">
+        <f>_xlfn.CONCAT(H21, $R$4)</f>
+        <v>BMK 3rd</v>
+      </c>
+      <c r="M21" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="11">
         <v>1.423</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O21" s="11">
         <v>1.43</v>
       </c>
-      <c r="P21" s="13">
+      <c r="P21" s="12">
         <v>1.4279999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M22" s="11" t="s">
+      <c r="A22" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="31"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="37"/>
+      <c r="M22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="11">
         <v>1.4279999999999999</v>
       </c>
-      <c r="O22" s="12">
+      <c r="O22" s="11">
         <v>1.42</v>
       </c>
-      <c r="P22" s="13">
+      <c r="P22" s="12">
         <v>1.4259999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M23" s="11" t="s">
+      <c r="A23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="37"/>
+      <c r="M23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N23" s="12">
+      <c r="N23" s="11">
         <v>1.381</v>
       </c>
-      <c r="O23" s="12">
+      <c r="O23" s="11">
         <v>1.373</v>
       </c>
-      <c r="P23" s="13">
+      <c r="P23" s="12">
         <v>1.38</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M24" s="11" t="s">
+      <c r="A24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="37"/>
+      <c r="M24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="N24" s="12">
+      <c r="N24" s="11">
         <v>1.4430000000000001</v>
       </c>
-      <c r="O24" s="12">
+      <c r="O24" s="11">
         <v>1.464</v>
       </c>
-      <c r="P24" s="13">
+      <c r="P24" s="12">
         <v>1.452</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M25" s="11" t="s">
+    <row r="25" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="38"/>
+      <c r="M25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N25" s="12">
+      <c r="N25" s="11">
         <v>1.405</v>
       </c>
-      <c r="O25" s="12">
+      <c r="O25" s="11">
         <v>1.3740000000000001</v>
       </c>
-      <c r="P25" s="13">
+      <c r="P25" s="12">
         <v>1.395</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M26" s="11" t="s">
+      <c r="M26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N26" s="12">
+      <c r="N26" s="11">
         <v>1.4119999999999999</v>
       </c>
-      <c r="O26" s="12">
+      <c r="O26" s="11">
         <v>1.407</v>
       </c>
-      <c r="P26" s="13">
+      <c r="P26" s="12">
         <v>1.41</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M27" s="11" t="s">
+      <c r="M27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N27" s="12">
+      <c r="N27" s="11">
         <v>1.397</v>
       </c>
-      <c r="O27" s="12">
+      <c r="O27" s="11">
         <v>1.4219999999999999</v>
       </c>
-      <c r="P27" s="13">
+      <c r="P27" s="12">
         <v>1.409</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="M28" s="16" t="s">
+      <c r="M28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N28" s="17">
+      <c r="N28" s="16">
         <v>1.0109999999999999</v>
       </c>
-      <c r="O28" s="17">
+      <c r="O28" s="16">
         <v>1.0109999999999999</v>
       </c>
-      <c r="P28" s="18">
+      <c r="P28" s="17">
         <v>1.014</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nov 18 changes, successful plots
</commit_message>
<xml_diff>
--- a/ComparisonQG.xlsx
+++ b/ComparisonQG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scaparas\.ssh\wwk-repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E79DB08-8F92-4567-9BA3-B53937CE7AB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D1A755-623D-4C7D-BDC1-52E6FE65F673}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -809,7 +809,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -906,6 +906,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -1314,7 +1320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1470,9 +1476,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1532,6 +1535,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1917,20 +1938,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.75" bestFit="1" customWidth="1"/>
@@ -2272,31 +2293,31 @@
       <c r="A10" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="71" t="s">
+      <c r="E10" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="F10" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="71" t="s">
+      <c r="G10" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="77" t="s">
+      <c r="H10" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="66" t="s">
+      <c r="I10" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="78" t="s">
+      <c r="J10" s="77" t="s">
         <v>43</v>
       </c>
       <c r="M10" s="8" t="s">
@@ -2316,32 +2337,32 @@
       <c r="A11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="66">
+      <c r="B11" s="65">
         <v>9.3920000000000003E-2</v>
       </c>
-      <c r="C11" s="69">
+      <c r="C11" s="68">
         <v>2.2950000000000002E-2</v>
       </c>
-      <c r="D11" s="85">
+      <c r="D11" s="84">
         <v>4.28E-3</v>
       </c>
-      <c r="E11" s="71">
+      <c r="E11" s="70">
         <v>5.1679999999999997E-2</v>
       </c>
-      <c r="F11" s="72">
+      <c r="F11" s="71">
         <v>2.3810000000000001E-2</v>
       </c>
-      <c r="G11" s="85">
+      <c r="G11" s="84">
         <v>2.2899999999999999E-3</v>
       </c>
-      <c r="H11" s="77">
+      <c r="H11" s="76">
         <v>5.0869999999999999E-2</v>
       </c>
-      <c r="I11" s="66">
+      <c r="I11" s="65">
         <f>$R$5 +  0.08867</f>
         <v>8.8679999999999995E-2</v>
       </c>
-      <c r="J11" s="79">
+      <c r="J11" s="78">
         <f>$R$5 + 0.05445</f>
         <v>5.4460000000000001E-2</v>
       </c>
@@ -2362,32 +2383,32 @@
       <c r="A12" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="68">
+      <c r="B12" s="67">
         <v>2.23264</v>
       </c>
-      <c r="C12" s="71">
+      <c r="C12" s="70">
         <v>2.2592300000000001</v>
       </c>
-      <c r="D12" s="71">
+      <c r="D12" s="70">
         <v>2.3289499999999999</v>
       </c>
-      <c r="E12" s="69">
+      <c r="E12" s="68">
         <v>2.2269800000000002</v>
       </c>
-      <c r="F12" s="71">
+      <c r="F12" s="70">
         <v>2.3082199999999999</v>
       </c>
-      <c r="G12" s="71">
+      <c r="G12" s="70">
         <v>2.5087100000000002</v>
       </c>
-      <c r="H12" s="77">
+      <c r="H12" s="76">
         <f>$R$5 + 2.19713</f>
         <v>2.1971400000000001</v>
       </c>
-      <c r="I12" s="66">
+      <c r="I12" s="65">
         <v>2.3877600000000001</v>
       </c>
-      <c r="J12" s="78">
+      <c r="J12" s="77">
         <v>2.5956399999999999</v>
       </c>
       <c r="M12" s="8" t="s">
@@ -2407,31 +2428,31 @@
       <c r="A13" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="75" t="s">
+      <c r="D13" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="76" t="s">
+      <c r="G13" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="74" t="s">
+      <c r="H13" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="73" t="s">
+      <c r="I13" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="80" t="s">
+      <c r="J13" s="79" t="s">
         <v>44</v>
       </c>
       <c r="M13" s="8" t="s">
@@ -2677,25 +2698,25 @@
       <c r="A22" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="81" t="str">
+      <c r="B22" s="80" t="str">
         <f>"La: " &amp;0.12089</f>
         <v>La: 0.12089</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="81" t="str">
+      <c r="E22" s="80" t="str">
         <f>"La: "&amp;ROUND(0.187050104442985, 5)</f>
         <v>La: 0.18705</v>
       </c>
-      <c r="F22" s="81" t="str">
+      <c r="F22" s="80" t="str">
         <f>"La: "&amp;ROUND(0.135447347517886, 5)</f>
         <v>La: 0.13545</v>
       </c>
-      <c r="G22" s="82" t="str">
+      <c r="G22" s="81" t="str">
         <f>"Lb: "&amp;ROUND(0.123883812132848, 5)</f>
         <v>Lb: 0.12388</v>
       </c>
@@ -2728,27 +2749,27 @@
       <c r="A23" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="81">
+      <c r="B23" s="80">
         <f>ROUND(0.1034202692, 5)</f>
         <v>0.10342</v>
       </c>
-      <c r="C23" s="82">
+      <c r="C23" s="81">
         <f>ROUND(0.0353096568, 5)</f>
         <v>3.5310000000000001E-2</v>
       </c>
-      <c r="D23" s="84">
+      <c r="D23" s="83">
         <f>ROUND(0.0021733422, 5)</f>
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="E23" s="82">
+      <c r="E23" s="81">
         <f>ROUND(0.0480188518, 5)</f>
         <v>4.802E-2</v>
       </c>
-      <c r="F23" s="81">
+      <c r="F23" s="80">
         <f>ROUND(0.0695032449, 5)</f>
         <v>6.9500000000000006E-2</v>
       </c>
-      <c r="G23" s="82">
+      <c r="G23" s="81">
         <f>ROUND(0.0122546477, 5)</f>
         <v>1.225E-2</v>
       </c>
@@ -2781,27 +2802,27 @@
       <c r="A24" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="82">
+      <c r="B24" s="81">
         <f>ROUND(2.25697841150508, 5)</f>
         <v>2.25698</v>
       </c>
-      <c r="C24" s="81">
+      <c r="C24" s="80">
         <f>ROUND(2.27012311119903, 5)</f>
         <v>2.2701199999999999</v>
       </c>
-      <c r="D24" s="81">
+      <c r="D24" s="80">
         <f>ROUND(2.2729670257177, 5)</f>
         <v>2.2729699999999999</v>
       </c>
-      <c r="E24" s="82">
+      <c r="E24" s="81">
         <f>ROUND(2.24728490850626, 5)</f>
         <v>2.2472799999999999</v>
       </c>
-      <c r="F24" s="81">
+      <c r="F24" s="80">
         <f>ROUND(2.51527310246819, 5)</f>
         <v>2.5152700000000001</v>
       </c>
-      <c r="G24" s="82">
+      <c r="G24" s="81">
         <f>ROUND(2.28160987024513, 5)</f>
         <v>2.2816100000000001</v>
       </c>
@@ -2834,22 +2855,22 @@
       <c r="A25" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="76" t="s">
+      <c r="D25" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="76" t="s">
+      <c r="E25" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="76" t="s">
+      <c r="F25" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="74" t="s">
+      <c r="G25" s="73" t="s">
         <v>34</v>
       </c>
       <c r="H25" s="41" t="s">
@@ -3147,27 +3168,27 @@
       <c r="A34" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="38" t="str">
+      <c r="B34" s="80" t="str">
         <f>"La: "&amp;ROUND(0.0923889163998217, 5)</f>
         <v>La: 0.09239</v>
       </c>
-      <c r="C34" s="38" t="str">
+      <c r="C34" s="81" t="str">
         <f>"Lb: "&amp;ROUND(0.0755745911359315, 5)</f>
         <v>Lb: 0.07557</v>
       </c>
-      <c r="D34" s="38" t="str">
+      <c r="D34" s="83" t="str">
         <f>"La: "&amp;ROUND(0.177571798227562, 5)</f>
         <v>La: 0.17757</v>
       </c>
-      <c r="E34" s="38" t="str">
+      <c r="E34" s="66" t="str">
         <f>"La: "&amp;ROUND(0.117252042408653, 5)</f>
         <v>La: 0.11725</v>
       </c>
-      <c r="F34" s="38" t="str">
+      <c r="F34" s="66" t="str">
         <f>"La: "&amp;ROUND(0.209717177548261, 5)</f>
         <v>La: 0.20972</v>
       </c>
-      <c r="G34" s="38" t="str">
+      <c r="G34" s="89" t="str">
         <f>"Lb: "&amp;ROUND(0.136102844114588, 5)</f>
         <v>Lb: 0.1361</v>
       </c>
@@ -3175,11 +3196,11 @@
         <f>"La: "&amp;ROUND(0.263197292471632, 5)</f>
         <v>La: 0.2632</v>
       </c>
-      <c r="I34" s="38" t="str">
+      <c r="I34" s="66" t="str">
         <f>"La: "&amp;ROUND(0.14083591567554, 5)</f>
         <v>La: 0.14084</v>
       </c>
-      <c r="J34" s="38" t="str">
+      <c r="J34" s="81" t="str">
         <f>"Lb: "&amp;ROUND(0.0923402242656354, 5)</f>
         <v>Lb: 0.09234</v>
       </c>
@@ -3188,27 +3209,27 @@
       <c r="A35" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B35" s="80">
         <f>ROUND(0.043112362, 5)</f>
         <v>4.3110000000000002E-2</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="81">
         <f>ROUND( 0.0176909199, 5)</f>
         <v>1.7690000000000001E-2</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="83">
         <f>ROUND(0.0012391746, 5)</f>
         <v>1.24E-3</v>
       </c>
-      <c r="E35" s="38">
+      <c r="E35" s="88">
         <f>ROUND(0.0019774986, 5)</f>
         <v>1.98E-3</v>
       </c>
-      <c r="F35" s="38">
+      <c r="F35" s="66">
         <f>ROUND(0.0019774986, 5)</f>
         <v>1.98E-3</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="88">
         <f>ROUND(0.0033135309, 5)</f>
         <v>3.31E-3</v>
       </c>
@@ -3216,11 +3237,11 @@
         <f>ROUND(0.0000035374, 5)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="38">
+      <c r="I35" s="81">
         <f>ROUND(0.0015486479, 5)</f>
         <v>1.5499999999999999E-3</v>
       </c>
-      <c r="J35" s="38">
+      <c r="J35" s="66">
         <f>ROUND(0.01063826, 5)</f>
         <v>1.064E-2</v>
       </c>
@@ -3229,27 +3250,27 @@
       <c r="A36" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="38">
+      <c r="B36" s="81">
         <f>ROUND(2.19818771946346, 5)</f>
         <v>2.1981899999999999</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="66">
         <f>ROUND(2.24287133380405, 5)</f>
         <v>2.2428699999999999</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="83">
         <f>ROUND(2.67043791352654, 5)</f>
         <v>2.6704400000000001</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="81">
         <f>ROUND(2.24941340797995, 5)</f>
         <v>2.2494100000000001</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="66">
         <f>ROUND(2.34291496431261, 5)</f>
         <v>2.3429099999999998</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="66">
         <f>ROUND(2.26402184618435, 5)</f>
         <v>2.2640199999999999</v>
       </c>
@@ -3257,11 +3278,11 @@
         <f>ROUND(3.01657346338523, 5)</f>
         <v>3.0165700000000002</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="81">
         <f>ROUND(2.22956241670871, 5)</f>
         <v>2.2295600000000002</v>
       </c>
-      <c r="J36" s="38">
+      <c r="J36" s="66">
         <f>ROUND(2.3049685681154, 5)</f>
         <v>2.30497</v>
       </c>
@@ -3270,31 +3291,31 @@
       <c r="A37" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="41" t="s">
+      <c r="D37" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="41" t="s">
+      <c r="E37" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="41" t="s">
+      <c r="F37" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="41" t="s">
+      <c r="G37" s="86" t="s">
         <v>35</v>
       </c>
       <c r="H37" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="I37" s="41" t="s">
+      <c r="I37" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="J37" s="65" t="s">
+      <c r="J37" s="90" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>